<commit_message>
Digital Marketing Lesson 14
</commit_message>
<xml_diff>
--- a/Lecture Completion Status.xlsx
+++ b/Lecture Completion Status.xlsx
@@ -1461,6 +1461,21 @@
     <xf numFmtId="164" fontId="9" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1476,19 +1491,19 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1521,20 +1536,68 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="14" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1542,15 +1605,6 @@
     <xf numFmtId="0" fontId="2" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1560,59 +1614,35 @@
     <xf numFmtId="0" fontId="2" fillId="20" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="14" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="23" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="23" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="23" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="22" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1623,9 +1653,6 @@
     <xf numFmtId="49" fontId="15" fillId="22" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1650,49 +1677,22 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="23" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="23" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="23" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2036,41 +2036,41 @@
     </row>
     <row r="2" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A2" s="14"/>
-      <c r="B2" s="128" t="s">
+      <c r="B2" s="123" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="128"/>
-      <c r="G2" s="128"/>
-      <c r="H2" s="128"/>
-      <c r="I2" s="128"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
       <c r="J2" s="15"/>
       <c r="K2" s="15"/>
     </row>
     <row r="3" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
-      <c r="B3" s="129" t="s">
+      <c r="B3" s="124" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="129" t="s">
+      <c r="C3" s="124" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="129" t="s">
+      <c r="D3" s="124" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="129"/>
-      <c r="F3" s="130" t="s">
+      <c r="E3" s="124"/>
+      <c r="F3" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="129" t="s">
+      <c r="G3" s="124" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="129" t="s">
+      <c r="H3" s="124" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="129" t="s">
+      <c r="I3" s="124" t="s">
         <v>6</v>
       </c>
       <c r="J3" s="15"/>
@@ -2078,18 +2078,18 @@
     </row>
     <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
-      <c r="B4" s="130"/>
-      <c r="C4" s="130"/>
+      <c r="B4" s="125"/>
+      <c r="C4" s="125"/>
       <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="131"/>
-      <c r="G4" s="130"/>
-      <c r="H4" s="129"/>
-      <c r="I4" s="129"/>
+      <c r="F4" s="126"/>
+      <c r="G4" s="125"/>
+      <c r="H4" s="124"/>
+      <c r="I4" s="124"/>
       <c r="J4" s="15"/>
       <c r="K4" s="15"/>
     </row>
@@ -2320,18 +2320,18 @@
     </row>
     <row r="13" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A13" s="14"/>
-      <c r="B13" s="127" t="s">
+      <c r="B13" s="122" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="127"/>
-      <c r="D13" s="127"/>
-      <c r="E13" s="127"/>
+      <c r="C13" s="122"/>
+      <c r="D13" s="122"/>
+      <c r="E13" s="122"/>
       <c r="F13" s="10"/>
-      <c r="G13" s="127" t="s">
+      <c r="G13" s="122" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="127"/>
-      <c r="I13" s="127"/>
+      <c r="H13" s="122"/>
+      <c r="I13" s="122"/>
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
     </row>
@@ -2353,10 +2353,10 @@
       <c r="G14" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="H14" s="126" t="s">
+      <c r="H14" s="131" t="s">
         <v>1</v>
       </c>
-      <c r="I14" s="126"/>
+      <c r="I14" s="131"/>
       <c r="J14" s="15"/>
       <c r="K14" s="15"/>
     </row>
@@ -2378,10 +2378,10 @@
       <c r="G15" s="12">
         <v>1</v>
       </c>
-      <c r="H15" s="122" t="s">
+      <c r="H15" s="127" t="s">
         <v>7</v>
       </c>
-      <c r="I15" s="123"/>
+      <c r="I15" s="128"/>
       <c r="J15" s="15"/>
       <c r="K15" s="15"/>
     </row>
@@ -2403,10 +2403,10 @@
       <c r="G16" s="9">
         <v>2</v>
       </c>
-      <c r="H16" s="124" t="s">
+      <c r="H16" s="129" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="125"/>
+      <c r="I16" s="130"/>
       <c r="J16" s="15"/>
       <c r="K16" s="15"/>
     </row>
@@ -2428,10 +2428,10 @@
       <c r="G17" s="12">
         <v>3</v>
       </c>
-      <c r="H17" s="122" t="s">
+      <c r="H17" s="127" t="s">
         <v>9</v>
       </c>
-      <c r="I17" s="123"/>
+      <c r="I17" s="128"/>
       <c r="J17" s="15"/>
       <c r="K17" s="15"/>
     </row>
@@ -2445,10 +2445,10 @@
       <c r="G18" s="9">
         <v>4</v>
       </c>
-      <c r="H18" s="124" t="s">
+      <c r="H18" s="129" t="s">
         <v>10</v>
       </c>
-      <c r="I18" s="125"/>
+      <c r="I18" s="130"/>
       <c r="J18" s="15"/>
       <c r="K18" s="15"/>
     </row>
@@ -2462,10 +2462,10 @@
       <c r="G19" s="12">
         <v>5</v>
       </c>
-      <c r="H19" s="122" t="s">
+      <c r="H19" s="127" t="s">
         <v>11</v>
       </c>
-      <c r="I19" s="123"/>
+      <c r="I19" s="128"/>
       <c r="J19" s="15"/>
       <c r="K19" s="15"/>
     </row>
@@ -2479,10 +2479,10 @@
       <c r="G20" s="9">
         <v>6</v>
       </c>
-      <c r="H20" s="124" t="s">
+      <c r="H20" s="129" t="s">
         <v>13</v>
       </c>
-      <c r="I20" s="125"/>
+      <c r="I20" s="130"/>
       <c r="J20" s="15"/>
       <c r="K20" s="15"/>
     </row>
@@ -3424,6 +3424,13 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="B2:I2"/>
@@ -3434,13 +3441,6 @@
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3480,56 +3480,56 @@
       <c r="J1" s="15"/>
     </row>
     <row r="2" spans="2:10" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B2" s="128" t="s">
+      <c r="B2" s="123" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="128"/>
-      <c r="G2" s="128"/>
-      <c r="H2" s="128"/>
-      <c r="I2" s="128"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
       <c r="J2" s="15"/>
     </row>
     <row r="3" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="129" t="s">
+      <c r="B3" s="124" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="129" t="s">
+      <c r="C3" s="124" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="129" t="s">
+      <c r="D3" s="124" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="129"/>
-      <c r="F3" s="139" t="s">
+      <c r="E3" s="124"/>
+      <c r="F3" s="144" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="129" t="s">
+      <c r="G3" s="124" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="129" t="s">
+      <c r="H3" s="124" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="129" t="s">
+      <c r="I3" s="124" t="s">
         <v>6</v>
       </c>
       <c r="J3" s="15"/>
     </row>
     <row r="4" spans="2:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="130"/>
-      <c r="C4" s="130"/>
+      <c r="B4" s="125"/>
+      <c r="C4" s="125"/>
       <c r="D4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="140"/>
-      <c r="G4" s="130"/>
-      <c r="H4" s="129"/>
-      <c r="I4" s="129"/>
+      <c r="F4" s="145"/>
+      <c r="G4" s="125"/>
+      <c r="H4" s="124"/>
+      <c r="I4" s="124"/>
       <c r="J4" s="15"/>
     </row>
     <row r="5" spans="2:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -3742,25 +3742,25 @@
       <c r="J12" s="15"/>
     </row>
     <row r="13" spans="2:10" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B13" s="127" t="s">
+      <c r="B13" s="122" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="127"/>
-      <c r="D13" s="127"/>
-      <c r="E13" s="127"/>
+      <c r="C13" s="122"/>
+      <c r="D13" s="122"/>
+      <c r="E13" s="122"/>
       <c r="F13" s="10"/>
-      <c r="G13" s="138" t="s">
+      <c r="G13" s="143" t="s">
         <v>38</v>
       </c>
-      <c r="H13" s="138"/>
-      <c r="I13" s="138"/>
+      <c r="H13" s="143"/>
+      <c r="I13" s="143"/>
       <c r="J13" s="15"/>
     </row>
     <row r="14" spans="2:10" s="15" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="141"/>
-      <c r="C14" s="141"/>
-      <c r="D14" s="141"/>
-      <c r="E14" s="141"/>
+      <c r="B14" s="146"/>
+      <c r="C14" s="146"/>
+      <c r="D14" s="146"/>
+      <c r="E14" s="146"/>
       <c r="F14" s="10"/>
       <c r="G14" s="40"/>
       <c r="H14" s="40"/>
@@ -3798,10 +3798,10 @@
       <c r="C16" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="142" t="s">
+      <c r="D16" s="135" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="143"/>
+      <c r="E16" s="136"/>
       <c r="F16" s="48"/>
       <c r="G16" s="34" t="s">
         <v>39</v>
@@ -3828,11 +3828,11 @@
         <v>6</v>
       </c>
       <c r="F17" s="48"/>
-      <c r="G17" s="136" t="s">
+      <c r="G17" s="141" t="s">
         <v>42</v>
       </c>
-      <c r="H17" s="137"/>
-      <c r="I17" s="137"/>
+      <c r="H17" s="142"/>
+      <c r="I17" s="142"/>
       <c r="J17" s="15"/>
     </row>
     <row r="18" spans="2:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3849,11 +3849,11 @@
         <v>3</v>
       </c>
       <c r="F18" s="48"/>
-      <c r="G18" s="145" t="s">
+      <c r="G18" s="133" t="s">
         <v>41</v>
       </c>
-      <c r="H18" s="146"/>
-      <c r="I18" s="146"/>
+      <c r="H18" s="134"/>
+      <c r="I18" s="134"/>
       <c r="J18" s="15"/>
     </row>
     <row r="19" spans="2:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3890,8 +3890,8 @@
       </c>
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
-      <c r="H20" s="144"/>
-      <c r="I20" s="144"/>
+      <c r="H20" s="132"/>
+      <c r="I20" s="132"/>
       <c r="J20" s="15"/>
     </row>
     <row r="21" spans="2:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3909,8 +3909,8 @@
       </c>
       <c r="F21" s="15"/>
       <c r="G21" s="15"/>
-      <c r="H21" s="144"/>
-      <c r="I21" s="144"/>
+      <c r="H21" s="132"/>
+      <c r="I21" s="132"/>
       <c r="J21" s="15"/>
     </row>
     <row r="22" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3920,10 +3920,10 @@
       <c r="C22" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="142" t="s">
+      <c r="D22" s="135" t="s">
         <v>32</v>
       </c>
-      <c r="E22" s="143"/>
+      <c r="E22" s="136"/>
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
@@ -3956,14 +3956,14 @@
       <c r="C24" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="142" t="s">
+      <c r="D24" s="135" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="143"/>
+      <c r="E24" s="136"/>
       <c r="F24" s="15"/>
       <c r="G24" s="19"/>
-      <c r="H24" s="144"/>
-      <c r="I24" s="144"/>
+      <c r="H24" s="132"/>
+      <c r="I24" s="132"/>
       <c r="J24" s="15"/>
     </row>
     <row r="25" spans="2:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3981,15 +3981,15 @@
       </c>
       <c r="F25" s="15"/>
       <c r="G25" s="19"/>
-      <c r="H25" s="144"/>
-      <c r="I25" s="144"/>
+      <c r="H25" s="132"/>
+      <c r="I25" s="132"/>
       <c r="J25" s="15"/>
     </row>
     <row r="26" spans="2:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="132" t="s">
+      <c r="B26" s="137" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="133"/>
+      <c r="C26" s="138"/>
       <c r="D26" s="22" t="s">
         <v>34</v>
       </c>
@@ -4003,8 +4003,8 @@
       <c r="J26" s="15"/>
     </row>
     <row r="27" spans="2:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="134"/>
-      <c r="C27" s="135"/>
+      <c r="B27" s="139"/>
+      <c r="C27" s="140"/>
       <c r="D27" s="45" t="s">
         <v>19</v>
       </c>
@@ -4032,8 +4032,8 @@
       </c>
       <c r="F28" s="15"/>
       <c r="G28" s="19"/>
-      <c r="H28" s="144"/>
-      <c r="I28" s="144"/>
+      <c r="H28" s="132"/>
+      <c r="I28" s="132"/>
       <c r="J28" s="15"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
@@ -4684,14 +4684,6 @@
     <row r="664" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H25:I25"/>
     <mergeCell ref="B26:C27"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="B13:E13"/>
@@ -4706,6 +4698,14 @@
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="D16:E16"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H25:I25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4746,56 +4746,56 @@
       <c r="J1" s="15"/>
     </row>
     <row r="2" spans="2:10" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B2" s="128" t="s">
+      <c r="B2" s="123" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="128"/>
-      <c r="G2" s="128"/>
-      <c r="H2" s="128"/>
-      <c r="I2" s="128"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
       <c r="J2" s="15"/>
     </row>
     <row r="3" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="129" t="s">
+      <c r="B3" s="124" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="129" t="s">
+      <c r="C3" s="124" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="129" t="s">
+      <c r="D3" s="124" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="129"/>
-      <c r="F3" s="139" t="s">
+      <c r="E3" s="124"/>
+      <c r="F3" s="144" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="129" t="s">
+      <c r="G3" s="124" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="129" t="s">
+      <c r="H3" s="124" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="129" t="s">
+      <c r="I3" s="124" t="s">
         <v>6</v>
       </c>
       <c r="J3" s="15"/>
     </row>
     <row r="4" spans="2:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="130"/>
-      <c r="C4" s="130"/>
+      <c r="B4" s="125"/>
+      <c r="C4" s="125"/>
       <c r="D4" s="51" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="140"/>
-      <c r="G4" s="130"/>
-      <c r="H4" s="129"/>
-      <c r="I4" s="129"/>
+      <c r="F4" s="145"/>
+      <c r="G4" s="125"/>
+      <c r="H4" s="124"/>
+      <c r="I4" s="124"/>
       <c r="J4" s="15"/>
     </row>
     <row r="5" spans="2:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -5008,18 +5008,18 @@
       <c r="J12" s="15"/>
     </row>
     <row r="13" spans="2:10" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B13" s="159" t="s">
+      <c r="B13" s="147" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="159"/>
-      <c r="D13" s="159"/>
-      <c r="E13" s="159"/>
+      <c r="C13" s="147"/>
+      <c r="D13" s="147"/>
+      <c r="E13" s="147"/>
       <c r="F13" s="10"/>
-      <c r="G13" s="159" t="s">
+      <c r="G13" s="147" t="s">
         <v>54</v>
       </c>
-      <c r="H13" s="159"/>
-      <c r="I13" s="159"/>
+      <c r="H13" s="147"/>
+      <c r="I13" s="147"/>
       <c r="J13" s="15"/>
     </row>
     <row r="14" spans="2:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -5036,11 +5036,11 @@
         <v>18</v>
       </c>
       <c r="F14" s="43"/>
-      <c r="G14" s="168" t="s">
+      <c r="G14" s="156" t="s">
         <v>55</v>
       </c>
-      <c r="H14" s="169"/>
-      <c r="I14" s="170"/>
+      <c r="H14" s="157"/>
+      <c r="I14" s="158"/>
       <c r="J14" s="15"/>
     </row>
     <row r="15" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -5057,11 +5057,11 @@
         <v>5</v>
       </c>
       <c r="F15" s="39"/>
-      <c r="G15" s="162" t="s">
+      <c r="G15" s="150" t="s">
         <v>57</v>
       </c>
-      <c r="H15" s="163"/>
-      <c r="I15" s="164"/>
+      <c r="H15" s="151"/>
+      <c r="I15" s="152"/>
       <c r="J15" s="15"/>
     </row>
     <row r="16" spans="2:10" s="15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -5078,11 +5078,11 @@
         <v>7</v>
       </c>
       <c r="F16" s="39"/>
-      <c r="G16" s="165" t="s">
+      <c r="G16" s="153" t="s">
         <v>56</v>
       </c>
-      <c r="H16" s="166"/>
-      <c r="I16" s="167"/>
+      <c r="H16" s="154"/>
+      <c r="I16" s="155"/>
     </row>
     <row r="17" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="60">
@@ -5117,11 +5117,11 @@
         <v>5</v>
       </c>
       <c r="F18" s="39"/>
-      <c r="G18" s="149" t="s">
+      <c r="G18" s="159" t="s">
         <v>63</v>
       </c>
-      <c r="H18" s="150"/>
-      <c r="I18" s="151"/>
+      <c r="H18" s="160"/>
+      <c r="I18" s="161"/>
     </row>
     <row r="19" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="61">
@@ -5137,11 +5137,11 @@
         <v>3</v>
       </c>
       <c r="F19" s="39"/>
-      <c r="G19" s="168" t="s">
+      <c r="G19" s="156" t="s">
         <v>64</v>
       </c>
-      <c r="H19" s="169"/>
-      <c r="I19" s="170"/>
+      <c r="H19" s="157"/>
+      <c r="I19" s="158"/>
       <c r="J19" s="15"/>
     </row>
     <row r="20" spans="2:10" s="15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -5166,25 +5166,25 @@
       <c r="C21" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="171" t="s">
+      <c r="D21" s="163" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="172"/>
+      <c r="E21" s="164"/>
       <c r="F21" s="39"/>
-      <c r="G21" s="149" t="s">
+      <c r="G21" s="159" t="s">
         <v>65</v>
       </c>
-      <c r="H21" s="150"/>
-      <c r="I21" s="151"/>
+      <c r="H21" s="160"/>
+      <c r="I21" s="161"/>
       <c r="J21" s="15"/>
     </row>
     <row r="22" spans="2:10" s="15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F22" s="39"/>
-      <c r="G22" s="124" t="s">
+      <c r="G22" s="129" t="s">
         <v>66</v>
       </c>
-      <c r="H22" s="155"/>
-      <c r="I22" s="125"/>
+      <c r="H22" s="162"/>
+      <c r="I22" s="130"/>
     </row>
     <row r="23" spans="2:10" s="15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="56"/>
@@ -5199,57 +5199,57 @@
       <c r="D24" s="19"/>
       <c r="E24" s="19"/>
       <c r="F24" s="39"/>
-      <c r="G24" s="149" t="s">
+      <c r="G24" s="159" t="s">
         <v>67</v>
       </c>
-      <c r="H24" s="150"/>
-      <c r="I24" s="151"/>
+      <c r="H24" s="160"/>
+      <c r="I24" s="161"/>
     </row>
     <row r="25" spans="2:10" s="15" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="160" t="s">
+      <c r="B25" s="148" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="161"/>
-      <c r="D25" s="161"/>
-      <c r="E25" s="161"/>
-      <c r="F25" s="161"/>
-      <c r="G25" s="152" t="s">
+      <c r="C25" s="149"/>
+      <c r="D25" s="149"/>
+      <c r="E25" s="149"/>
+      <c r="F25" s="149"/>
+      <c r="G25" s="170" t="s">
         <v>68</v>
       </c>
-      <c r="H25" s="153"/>
-      <c r="I25" s="154"/>
+      <c r="H25" s="171"/>
+      <c r="I25" s="172"/>
     </row>
     <row r="26" spans="2:10" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="147" t="s">
+      <c r="B26" s="168" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="147"/>
-      <c r="D26" s="147"/>
-      <c r="E26" s="147"/>
-      <c r="F26" s="147"/>
-      <c r="G26" s="124" t="s">
+      <c r="C26" s="168"/>
+      <c r="D26" s="168"/>
+      <c r="E26" s="168"/>
+      <c r="F26" s="168"/>
+      <c r="G26" s="129" t="s">
         <v>69</v>
       </c>
-      <c r="H26" s="155"/>
-      <c r="I26" s="125"/>
+      <c r="H26" s="162"/>
+      <c r="I26" s="130"/>
     </row>
     <row r="27" spans="2:10" s="15" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="148" t="s">
+      <c r="B27" s="169" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="148"/>
-      <c r="D27" s="148"/>
-      <c r="E27" s="148"/>
-      <c r="F27" s="148"/>
+      <c r="C27" s="169"/>
+      <c r="D27" s="169"/>
+      <c r="E27" s="169"/>
+      <c r="F27" s="169"/>
     </row>
     <row r="28" spans="2:10" s="15" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="157" t="s">
+      <c r="C28" s="166" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="157"/>
+      <c r="D28" s="166"/>
       <c r="E28" s="65" t="s">
         <v>17</v>
       </c>
@@ -5261,10 +5261,10 @@
       <c r="B29" s="58">
         <v>45516</v>
       </c>
-      <c r="C29" s="158" t="s">
+      <c r="C29" s="167" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="158"/>
+      <c r="D29" s="167"/>
       <c r="E29" s="59" t="s">
         <v>50</v>
       </c>
@@ -5276,10 +5276,10 @@
       <c r="B30" s="58">
         <v>45517</v>
       </c>
-      <c r="C30" s="158" t="s">
+      <c r="C30" s="167" t="s">
         <v>53</v>
       </c>
-      <c r="D30" s="158"/>
+      <c r="D30" s="167"/>
       <c r="E30" s="59" t="s">
         <v>50</v>
       </c>
@@ -5290,8 +5290,8 @@
     <row r="31" spans="2:10" s="15" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="2:10" s="15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G32" s="19"/>
-      <c r="H32" s="144"/>
-      <c r="I32" s="144"/>
+      <c r="H32" s="132"/>
+      <c r="I32" s="132"/>
     </row>
     <row r="33" spans="2:9" s="15" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="53"/>
@@ -5299,12 +5299,12 @@
       <c r="D33" s="19"/>
       <c r="E33" s="19"/>
       <c r="G33" s="19"/>
-      <c r="H33" s="144"/>
-      <c r="I33" s="144"/>
+      <c r="H33" s="132"/>
+      <c r="I33" s="132"/>
     </row>
     <row r="34" spans="2:9" s="15" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="156"/>
-      <c r="C34" s="156"/>
+      <c r="B34" s="165"/>
+      <c r="C34" s="165"/>
       <c r="D34" s="19"/>
       <c r="E34" s="19"/>
       <c r="G34" s="19"/>
@@ -5312,8 +5312,8 @@
       <c r="I34" s="52"/>
     </row>
     <row r="35" spans="2:9" s="15" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="156"/>
-      <c r="C35" s="156"/>
+      <c r="B35" s="165"/>
+      <c r="C35" s="165"/>
       <c r="D35" s="54"/>
       <c r="E35" s="54"/>
       <c r="G35" s="19"/>
@@ -5322,8 +5322,8 @@
     </row>
     <row r="36" spans="2:9" s="15" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G36" s="19"/>
-      <c r="H36" s="144"/>
-      <c r="I36" s="144"/>
+      <c r="H36" s="132"/>
+      <c r="I36" s="132"/>
     </row>
     <row r="37" spans="2:9" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="2:9" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -5963,6 +5963,26 @@
     <row r="672" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="B34:C35"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="B25:F25"/>
@@ -5974,26 +5994,6 @@
     <mergeCell ref="G22:I22"/>
     <mergeCell ref="G18:I18"/>
     <mergeCell ref="D21:E21"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="B34:C35"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G26:I26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6027,17 +6027,17 @@
     <row r="1" spans="1:17" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:17" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A2" s="14"/>
-      <c r="B2" s="128" t="s">
+      <c r="B2" s="123" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="128"/>
-      <c r="G2" s="128"/>
-      <c r="H2" s="128"/>
-      <c r="I2" s="128"/>
-      <c r="J2" s="128"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
+      <c r="J2" s="123"/>
       <c r="K2" s="15"/>
       <c r="L2" s="15"/>
       <c r="P2"/>
@@ -6045,27 +6045,27 @@
     </row>
     <row r="3" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
-      <c r="B3" s="129" t="s">
+      <c r="B3" s="124" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="129" t="s">
+      <c r="C3" s="124" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="129" t="s">
+      <c r="D3" s="124" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="129"/>
-      <c r="F3" s="177" t="s">
+      <c r="E3" s="124"/>
+      <c r="F3" s="186" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="178"/>
-      <c r="H3" s="129" t="s">
+      <c r="G3" s="187"/>
+      <c r="H3" s="124" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="129" t="s">
+      <c r="I3" s="124" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="129" t="s">
+      <c r="J3" s="124" t="s">
         <v>6</v>
       </c>
       <c r="K3" s="15"/>
@@ -6075,19 +6075,19 @@
     </row>
     <row r="4" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
-      <c r="B4" s="130"/>
-      <c r="C4" s="130"/>
+      <c r="B4" s="125"/>
+      <c r="C4" s="125"/>
       <c r="D4" s="80" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="179"/>
-      <c r="G4" s="180"/>
-      <c r="H4" s="130"/>
-      <c r="I4" s="129"/>
-      <c r="J4" s="129"/>
+      <c r="F4" s="188"/>
+      <c r="G4" s="189"/>
+      <c r="H4" s="125"/>
+      <c r="I4" s="124"/>
+      <c r="J4" s="124"/>
       <c r="K4" s="15"/>
       <c r="L4" s="15"/>
       <c r="P4"/>
@@ -6107,10 +6107,10 @@
       <c r="E5" s="6">
         <v>12</v>
       </c>
-      <c r="F5" s="181">
+      <c r="F5" s="190">
         <v>3</v>
       </c>
-      <c r="G5" s="182"/>
+      <c r="G5" s="191"/>
       <c r="H5" s="6">
         <f>E5*F5</f>
         <v>36</v>
@@ -6149,31 +6149,31 @@
         <v>45</v>
       </c>
       <c r="F7" s="54"/>
-      <c r="G7" s="183" t="s">
+      <c r="G7" s="192" t="s">
         <v>80</v>
       </c>
-      <c r="H7" s="161"/>
-      <c r="I7" s="161"/>
-      <c r="J7" s="161"/>
+      <c r="H7" s="149"/>
+      <c r="I7" s="149"/>
+      <c r="J7" s="149"/>
       <c r="K7" s="71"/>
       <c r="L7" s="71"/>
     </row>
     <row r="8" spans="1:17" s="15" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B8" s="159" t="s">
+      <c r="B8" s="147" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="159"/>
-      <c r="D8" s="159"/>
-      <c r="E8" s="185"/>
+      <c r="C8" s="147"/>
+      <c r="D8" s="147"/>
+      <c r="E8" s="182"/>
       <c r="F8" s="81"/>
       <c r="G8" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="184" t="s">
+      <c r="H8" s="193" t="s">
         <v>81</v>
       </c>
-      <c r="I8" s="184"/>
-      <c r="J8" s="184"/>
+      <c r="I8" s="193"/>
+      <c r="J8" s="193"/>
       <c r="K8" s="72"/>
     </row>
     <row r="9" spans="1:17" s="15" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -6193,11 +6193,11 @@
       <c r="G9" s="75" t="s">
         <v>82</v>
       </c>
-      <c r="H9" s="176" t="s">
+      <c r="H9" s="173" t="s">
         <v>90</v>
       </c>
-      <c r="I9" s="176"/>
-      <c r="J9" s="176"/>
+      <c r="I9" s="173"/>
+      <c r="J9" s="173"/>
       <c r="K9" s="62"/>
     </row>
     <row r="10" spans="1:17" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -6217,11 +6217,11 @@
       <c r="G10" s="75" t="s">
         <v>83</v>
       </c>
-      <c r="H10" s="176" t="s">
+      <c r="H10" s="173" t="s">
         <v>91</v>
       </c>
-      <c r="I10" s="176"/>
-      <c r="J10" s="176"/>
+      <c r="I10" s="173"/>
+      <c r="J10" s="173"/>
       <c r="K10" s="62"/>
     </row>
     <row r="11" spans="1:17" s="15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -6241,11 +6241,11 @@
       <c r="G11" s="75" t="s">
         <v>84</v>
       </c>
-      <c r="H11" s="176" t="s">
+      <c r="H11" s="173" t="s">
         <v>92</v>
       </c>
-      <c r="I11" s="176"/>
-      <c r="J11" s="176"/>
+      <c r="I11" s="173"/>
+      <c r="J11" s="173"/>
       <c r="K11" s="62"/>
     </row>
     <row r="12" spans="1:17" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -6265,11 +6265,11 @@
       <c r="G12" s="75" t="s">
         <v>85</v>
       </c>
-      <c r="H12" s="176" t="s">
+      <c r="H12" s="173" t="s">
         <v>93</v>
       </c>
-      <c r="I12" s="176"/>
-      <c r="J12" s="176"/>
+      <c r="I12" s="173"/>
+      <c r="J12" s="173"/>
       <c r="K12" s="62"/>
     </row>
     <row r="13" spans="1:17" s="15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
@@ -6279,19 +6279,19 @@
       <c r="C13" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="171" t="s">
+      <c r="D13" s="163" t="s">
         <v>87</v>
       </c>
-      <c r="E13" s="172"/>
+      <c r="E13" s="164"/>
       <c r="F13" s="57"/>
       <c r="G13" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="H13" s="176" t="s">
+      <c r="H13" s="173" t="s">
         <v>94</v>
       </c>
-      <c r="I13" s="176"/>
-      <c r="J13" s="176"/>
+      <c r="I13" s="173"/>
+      <c r="J13" s="173"/>
       <c r="K13" s="72"/>
     </row>
     <row r="14" spans="1:17" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -6311,11 +6311,11 @@
       <c r="G14" s="77" t="s">
         <v>88</v>
       </c>
-      <c r="H14" s="173" t="s">
+      <c r="H14" s="183" t="s">
         <v>98</v>
       </c>
-      <c r="I14" s="174"/>
-      <c r="J14" s="175"/>
+      <c r="I14" s="184"/>
+      <c r="J14" s="185"/>
       <c r="K14" s="62"/>
     </row>
     <row r="15" spans="1:17" s="15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -6335,11 +6335,11 @@
       <c r="G15" s="76" t="s">
         <v>89</v>
       </c>
-      <c r="H15" s="176" t="s">
+      <c r="H15" s="173" t="s">
         <v>95</v>
       </c>
-      <c r="I15" s="176"/>
-      <c r="J15" s="176"/>
+      <c r="I15" s="173"/>
+      <c r="J15" s="173"/>
       <c r="K15" s="39"/>
     </row>
     <row r="16" spans="1:17" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -6349,19 +6349,19 @@
       <c r="C16" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="186" t="s">
+      <c r="D16" s="174" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="187"/>
+      <c r="E16" s="175"/>
       <c r="F16" s="82"/>
       <c r="G16" s="78" t="s">
         <v>89</v>
       </c>
-      <c r="H16" s="188" t="s">
+      <c r="H16" s="176" t="s">
         <v>97</v>
       </c>
-      <c r="I16" s="189"/>
-      <c r="J16" s="190"/>
+      <c r="I16" s="177"/>
+      <c r="J16" s="178"/>
       <c r="K16" s="74"/>
     </row>
     <row r="17" spans="2:11" s="15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -6381,11 +6381,11 @@
       <c r="G17" s="79" t="s">
         <v>86</v>
       </c>
-      <c r="H17" s="191" t="s">
+      <c r="H17" s="179" t="s">
         <v>96</v>
       </c>
-      <c r="I17" s="192"/>
-      <c r="J17" s="193"/>
+      <c r="I17" s="180"/>
+      <c r="J17" s="181"/>
       <c r="K17" s="39"/>
     </row>
     <row r="18" spans="2:11" s="15" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6404,36 +6404,36 @@
       <c r="G18" s="76" t="s">
         <v>99</v>
       </c>
-      <c r="H18" s="176" t="s">
+      <c r="H18" s="173" t="s">
         <v>100</v>
       </c>
-      <c r="I18" s="176"/>
-      <c r="J18" s="176"/>
+      <c r="I18" s="173"/>
+      <c r="J18" s="173"/>
     </row>
     <row r="19" spans="2:11" s="15" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G19" s="76" t="s">
         <v>101</v>
       </c>
-      <c r="H19" s="176" t="s">
+      <c r="H19" s="173" t="s">
         <v>102</v>
       </c>
-      <c r="I19" s="176"/>
-      <c r="J19" s="176"/>
+      <c r="I19" s="173"/>
+      <c r="J19" s="173"/>
     </row>
     <row r="20" spans="2:11" s="15" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="127" t="s">
+      <c r="B20" s="122" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="127"/>
-      <c r="D20" s="127"/>
+      <c r="C20" s="122"/>
+      <c r="D20" s="122"/>
       <c r="G20" s="76" t="s">
         <v>103</v>
       </c>
-      <c r="H20" s="176" t="s">
+      <c r="H20" s="173" t="s">
         <v>104</v>
       </c>
-      <c r="I20" s="176"/>
-      <c r="J20" s="176"/>
+      <c r="I20" s="173"/>
+      <c r="J20" s="173"/>
     </row>
     <row r="21" spans="2:11" s="15" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="89" t="s">
@@ -6446,11 +6446,11 @@
       <c r="G21" s="76" t="s">
         <v>105</v>
       </c>
-      <c r="H21" s="176" t="s">
+      <c r="H21" s="173" t="s">
         <v>106</v>
       </c>
-      <c r="I21" s="176"/>
-      <c r="J21" s="176"/>
+      <c r="I21" s="173"/>
+      <c r="J21" s="173"/>
     </row>
     <row r="22" spans="2:11" s="15" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="12">
@@ -6463,51 +6463,51 @@
       <c r="G22" s="76" t="s">
         <v>107</v>
       </c>
-      <c r="H22" s="176" t="s">
+      <c r="H22" s="173" t="s">
         <v>108</v>
       </c>
-      <c r="I22" s="176"/>
-      <c r="J22" s="176"/>
+      <c r="I22" s="173"/>
+      <c r="J22" s="173"/>
     </row>
     <row r="23" spans="2:11" s="15" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G23" s="76" t="s">
         <v>109</v>
       </c>
-      <c r="H23" s="176" t="s">
+      <c r="H23" s="173" t="s">
         <v>110</v>
       </c>
-      <c r="I23" s="176"/>
-      <c r="J23" s="176"/>
+      <c r="I23" s="173"/>
+      <c r="J23" s="173"/>
     </row>
     <row r="24" spans="2:11" s="15" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G24" s="76" t="s">
         <v>112</v>
       </c>
-      <c r="H24" s="176" t="s">
+      <c r="H24" s="173" t="s">
         <v>113</v>
       </c>
-      <c r="I24" s="176"/>
-      <c r="J24" s="176"/>
+      <c r="I24" s="173"/>
+      <c r="J24" s="173"/>
     </row>
     <row r="25" spans="2:11" s="15" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G25" s="76" t="s">
         <v>114</v>
       </c>
-      <c r="H25" s="176" t="s">
+      <c r="H25" s="173" t="s">
         <v>115</v>
       </c>
-      <c r="I25" s="176"/>
-      <c r="J25" s="176"/>
+      <c r="I25" s="173"/>
+      <c r="J25" s="173"/>
     </row>
     <row r="26" spans="2:11" s="15" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G26" s="76" t="s">
         <v>116</v>
       </c>
-      <c r="H26" s="176" t="s">
+      <c r="H26" s="173" t="s">
         <v>117</v>
       </c>
-      <c r="I26" s="176"/>
-      <c r="J26" s="176"/>
+      <c r="I26" s="173"/>
+      <c r="J26" s="173"/>
     </row>
     <row r="27" spans="2:11" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="2:11" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -7112,6 +7112,26 @@
     <row r="627" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="F3:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
     <mergeCell ref="H26:J26"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="B20:D20"/>
@@ -7125,26 +7145,6 @@
     <mergeCell ref="H21:J21"/>
     <mergeCell ref="H22:J22"/>
     <mergeCell ref="H23:J23"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="F3:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="G7:J7"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="H9:J9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7156,7 +7156,7 @@
   <dimension ref="A1:Q621"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H12" sqref="H12:J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7178,17 +7178,17 @@
     <row r="1" spans="1:17" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:17" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A2" s="14"/>
-      <c r="B2" s="128" t="s">
+      <c r="B2" s="123" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="128"/>
-      <c r="G2" s="128"/>
-      <c r="H2" s="128"/>
-      <c r="I2" s="128"/>
-      <c r="J2" s="128"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
+      <c r="J2" s="123"/>
       <c r="K2" s="15"/>
       <c r="L2" s="15"/>
       <c r="P2"/>
@@ -7196,27 +7196,27 @@
     </row>
     <row r="3" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
-      <c r="B3" s="129" t="s">
+      <c r="B3" s="124" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="129" t="s">
+      <c r="C3" s="124" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="129" t="s">
+      <c r="D3" s="124" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="129"/>
-      <c r="F3" s="177" t="s">
+      <c r="E3" s="124"/>
+      <c r="F3" s="186" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="178"/>
-      <c r="H3" s="129" t="s">
+      <c r="G3" s="187"/>
+      <c r="H3" s="124" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="129" t="s">
+      <c r="I3" s="124" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="129" t="s">
+      <c r="J3" s="124" t="s">
         <v>6</v>
       </c>
       <c r="K3" s="15"/>
@@ -7226,19 +7226,19 @@
     </row>
     <row r="4" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
-      <c r="B4" s="130"/>
-      <c r="C4" s="130"/>
+      <c r="B4" s="125"/>
+      <c r="C4" s="125"/>
       <c r="D4" s="92" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="179"/>
-      <c r="G4" s="180"/>
-      <c r="H4" s="130"/>
-      <c r="I4" s="129"/>
-      <c r="J4" s="129"/>
+      <c r="F4" s="188"/>
+      <c r="G4" s="189"/>
+      <c r="H4" s="125"/>
+      <c r="I4" s="124"/>
+      <c r="J4" s="124"/>
       <c r="K4" s="15"/>
       <c r="L4" s="15"/>
       <c r="P4"/>
@@ -7258,20 +7258,20 @@
       <c r="E5" s="6">
         <v>12</v>
       </c>
-      <c r="F5" s="181">
+      <c r="F5" s="190">
         <v>3</v>
       </c>
-      <c r="G5" s="182"/>
+      <c r="G5" s="191"/>
       <c r="H5" s="6">
         <f>E5*F5</f>
         <v>36</v>
       </c>
       <c r="I5" s="6">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J5" s="6">
         <f t="shared" ref="J5" si="0">H5-I5</f>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K5" s="15"/>
       <c r="L5" s="15"/>
@@ -7300,31 +7300,31 @@
         <v>45</v>
       </c>
       <c r="F7" s="54"/>
-      <c r="G7" s="183" t="s">
+      <c r="G7" s="192" t="s">
         <v>80</v>
       </c>
-      <c r="H7" s="161"/>
-      <c r="I7" s="161"/>
-      <c r="J7" s="161"/>
+      <c r="H7" s="149"/>
+      <c r="I7" s="149"/>
+      <c r="J7" s="149"/>
       <c r="K7" s="71"/>
       <c r="L7" s="71"/>
     </row>
     <row r="8" spans="1:17" s="15" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B8" s="159" t="s">
+      <c r="B8" s="147" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="159"/>
-      <c r="D8" s="159"/>
-      <c r="E8" s="185"/>
+      <c r="C8" s="147"/>
+      <c r="D8" s="147"/>
+      <c r="E8" s="182"/>
       <c r="F8" s="93"/>
       <c r="G8" s="95" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="184" t="s">
+      <c r="H8" s="193" t="s">
         <v>81</v>
       </c>
-      <c r="I8" s="184"/>
-      <c r="J8" s="184"/>
+      <c r="I8" s="193"/>
+      <c r="J8" s="193"/>
       <c r="K8" s="72"/>
     </row>
     <row r="9" spans="1:17" s="15" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -7344,11 +7344,11 @@
       <c r="G9" s="75" t="s">
         <v>121</v>
       </c>
-      <c r="H9" s="176" t="s">
+      <c r="H9" s="173" t="s">
         <v>120</v>
       </c>
-      <c r="I9" s="176"/>
-      <c r="J9" s="176"/>
+      <c r="I9" s="173"/>
+      <c r="J9" s="173"/>
       <c r="K9" s="62"/>
     </row>
     <row r="10" spans="1:17" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -7368,11 +7368,11 @@
       <c r="G10" s="75" t="s">
         <v>122</v>
       </c>
-      <c r="H10" s="176" t="s">
+      <c r="H10" s="173" t="s">
         <v>123</v>
       </c>
-      <c r="I10" s="176"/>
-      <c r="J10" s="176"/>
+      <c r="I10" s="173"/>
+      <c r="J10" s="173"/>
       <c r="K10" s="62"/>
     </row>
     <row r="11" spans="1:17" s="15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -7388,11 +7388,11 @@
       <c r="G11" s="75" t="s">
         <v>125</v>
       </c>
-      <c r="H11" s="176" t="s">
+      <c r="H11" s="173" t="s">
         <v>124</v>
       </c>
-      <c r="I11" s="176"/>
-      <c r="J11" s="176"/>
+      <c r="I11" s="173"/>
+      <c r="J11" s="173"/>
       <c r="K11" s="62"/>
     </row>
     <row r="12" spans="1:17" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -7418,8 +7418,8 @@
       <c r="C13" s="117" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="198"/>
-      <c r="E13" s="199"/>
+      <c r="D13" s="195"/>
+      <c r="E13" s="196"/>
       <c r="F13" s="57"/>
       <c r="G13" s="114"/>
       <c r="H13" s="194"/>
@@ -7466,8 +7466,8 @@
       <c r="C16" s="121" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="195"/>
-      <c r="E16" s="196"/>
+      <c r="D16" s="198"/>
+      <c r="E16" s="199"/>
       <c r="F16" s="82"/>
       <c r="G16" s="114"/>
       <c r="H16" s="197"/>
@@ -8125,14 +8125,12 @@
     <row r="621" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="H18:J18"/>
     <mergeCell ref="H15:J15"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="G7:J7"/>
@@ -8145,12 +8143,14 @@
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="H13:J13"/>
     <mergeCell ref="H14:J14"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>